<commit_message>
Updating MALDI and SIMS for field name changes
</commit_message>
<xml_diff>
--- a/maldi/latest/maldi.xlsx
+++ b/maldi/latest/maldi.xlsx
@@ -14,10 +14,10 @@
     <sheet name="acquisition_instrument_model" r:id="rId8" sheetId="6"/>
     <sheet name="source_storage_duration_unit" r:id="rId9" sheetId="7"/>
     <sheet name="time_since_acquisition_instrume" r:id="rId10" sheetId="8"/>
-    <sheet name="mass_spectrometry_ionization_te" r:id="rId11" sheetId="9"/>
-    <sheet name="mass_analysis_polarity" r:id="rId12" sheetId="10"/>
-    <sheet name="ion_mobility" r:id="rId13" sheetId="11"/>
-    <sheet name="mass_spectrometry_scan_mode" r:id="rId14" sheetId="12"/>
+    <sheet name="ms_ionization_technique" r:id="rId11" sheetId="9"/>
+    <sheet name="ms_scan_mode" r:id="rId12" sheetId="10"/>
+    <sheet name="mass_analysis_polarity" r:id="rId13" sheetId="11"/>
+    <sheet name="ion_mobility" r:id="rId14" sheetId="12"/>
     <sheet name="matrix_deposition_method" r:id="rId15" sheetId="13"/>
     <sheet name="preparation_instrument_vendor" r:id="rId16" sheetId="14"/>
     <sheet name="preparation_instrument_model" r:id="rId17" sheetId="15"/>
@@ -145,32 +145,38 @@
     </comment>
     <comment ref="P1" authorId="1">
       <text>
-        <t>(Required) The polarity of the mass analysis (positive or negative ion modes).</t>
+        <t>(Required) MS (mass spectrometry) scan mode refers to the number of steps in the
+separation of fragments.</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="1">
       <text>
-        <t>(Required) The low value of the scanned mass range. (unitless)</t>
+        <t>(Required) The polarity of the mass analysis (positive or negative ion modes).</t>
       </text>
     </comment>
     <comment ref="R1" authorId="1">
       <text>
-        <t>(Required) The high value of the scanned mass range. (unitless)</t>
+        <t>The low value of the scanned mass-to-charge range, for MS1. (unitless)</t>
       </text>
     </comment>
     <comment ref="S1" authorId="1">
+      <text>
+        <t>The high value of the scanned mass-to-charge range, for MS1. (unitless)</t>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="1">
       <text>
         <t>(Required) The mass resolving power m/∆m, where ∆m is defined as the full width
 at half-maximum (FWHM) for a given peak with a specified mass-to-charge (m/z).
 (unitless)</t>
       </text>
     </comment>
-    <comment ref="T1" authorId="1">
+    <comment ref="U1" authorId="1">
       <text>
         <t>(Required) The peak (m/z) used to calculate the resolving power.</t>
       </text>
     </comment>
-    <comment ref="U1" authorId="1">
+    <comment ref="V1" authorId="1">
       <text>
         <t>Specifies which technology was used for ion mobility spectrometry. Technologies
 for measuring ion mobility: Traveling Wave Ion Mobility Spectrometry (TWIMS),
@@ -178,12 +184,6 @@
 Mobility Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS),
 Structures for Lossless Ion Manipulations (SLIM), and cyclic Ion Mobility
 Spectrometry (cIMS).</t>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="1">
-      <text>
-        <t>(Required) Scan mode refers to the number of steps in the separation of
-fragments.</t>
       </text>
     </comment>
     <comment ref="W1" authorId="1">
@@ -216,6 +216,13 @@
     </comment>
     <comment ref="AA1" authorId="1">
       <text>
+        <t>(Required) A DOI to a protocols.io protocol describing the software and
+database(s) used to process the raw data. Example:
+https://dx.doi.org/10.17504/protocols.io.bsu5ney6</t>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="1">
+      <text>
         <t>(Required) The string that serves as the definitive identifier for the metadata
 schema version and is readily interpretable by computers for data validation and
 processing. Example: 22bc762a-5020-419d-b170-24253ed9e8d9</t>
@@ -226,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="332">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -888,7 +895,7 @@
     <t>data_path</t>
   </si>
   <si>
-    <t>mass_spectrometry_ionization_technique</t>
+    <t>ms_ionization_technique</t>
   </si>
   <si>
     <t>LDI</t>
@@ -933,6 +940,27 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000279</t>
   </si>
   <si>
+    <t>ms_scan_mode</t>
+  </si>
+  <si>
+    <t>MS3</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000230</t>
+  </si>
+  <si>
+    <t>MS2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000229</t>
+  </si>
+  <si>
+    <t>MS1</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000228</t>
+  </si>
+  <si>
     <t>mass_analysis_polarity</t>
   </si>
   <si>
@@ -1005,27 +1033,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000224</t>
   </si>
   <si>
-    <t>mass_spectrometry_scan_mode</t>
-  </si>
-  <si>
-    <t>MS3</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000230</t>
-  </si>
-  <si>
-    <t>MS2</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000229</t>
-  </si>
-  <si>
-    <t>MS1</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000228</t>
-  </si>
-  <si>
     <t>matrix_deposition_method</t>
   </si>
   <si>
@@ -1194,6 +1201,9 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_64340</t>
   </si>
   <si>
+    <t>analysis_protocol_doi</t>
+  </si>
+  <si>
     <t>metadata_schema_id</t>
   </si>
   <si>
@@ -1212,7 +1222,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2023-10-16T20:50:47-07:00</t>
+    <t>2023-10-18T12:04:03-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1271,7 +1281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyAlignment="true" applyFill="true">
       <alignment horizontal="center"/>
@@ -1287,6 +1297,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1313,7 +1324,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1333,19 +1344,20 @@
     <col min="12" max="12" style="13" width="46.48828125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" style="14" width="16.90625" customWidth="true" bestFit="true"/>
     <col min="14" max="14" style="15" width="9.81640625" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" style="16" width="37.7578125" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" style="17" width="21.265625" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" style="18" width="30.8203125" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" style="19" width="31.69921875" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" style="20" width="21.0546875" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" style="21" width="30.70703125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" style="22" width="11.98046875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" style="23" width="29.16015625" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" style="16" width="23.15625" customWidth="true" bestFit="true"/>
+    <col min="16" max="16" style="17" width="14.55859375" customWidth="true" bestFit="true"/>
+    <col min="17" max="17" style="18" width="21.265625" customWidth="true" bestFit="true"/>
+    <col min="18" max="18" style="19" width="30.8203125" customWidth="true" bestFit="true"/>
+    <col min="19" max="19" style="20" width="31.69921875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" style="21" width="21.0546875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" style="22" width="30.70703125" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" style="23" width="11.98046875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" style="24" width="24.92578125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" style="25" width="29.08203125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" style="26" width="28.48828125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" style="27" width="18.109375" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" style="28" width="19.61328125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" style="28" width="20.17578125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" style="29" width="19.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1401,19 +1413,19 @@
         <v>242</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="W1" t="s" s="1">
         <v>266</v>
@@ -1430,10 +1442,13 @@
       <c r="AA1" t="s" s="1">
         <v>322</v>
       </c>
+      <c r="AB1" t="s" s="1">
+        <v>323</v>
+      </c>
     </row>
     <row r="2">
-      <c r="AA2" t="s">
-        <v>323</v>
+      <c r="AB2" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -1468,14 +1483,13 @@
       <formula1>'time_since_acquisition_instrument_calibration_unit'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="O2:O1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'mass_spectrometry_ionization_technique'!$A$1:$A$8</formula1>
+      <formula1>'ms_ionization_technique'!$A$1:$A$8</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="P2:P1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
+      <formula1>'ms_scan_mode'!$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'mass_analysis_polarity'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="between" sqref="Q2:Q1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
-      <formula1>-3.4028235E38</formula1>
-      <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="decimal" operator="between" sqref="R2:R1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
       <formula1>-3.4028235E38</formula1>
@@ -1489,11 +1503,12 @@
       <formula1>-3.4028235E38</formula1>
       <formula2>3.4028235E38</formula2>
     </dataValidation>
-    <dataValidation type="list" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'ion_mobility'!$A$1:$A$6</formula1>
+    <dataValidation type="decimal" operator="between" sqref="U2:U1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be a number" showErrorMessage="true">
+      <formula1>-3.4028235E38</formula1>
+      <formula2>3.4028235E38</formula2>
     </dataValidation>
     <dataValidation type="list" sqref="V2:V1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'mass_spectrometry_scan_mode'!$A$1:$A$3</formula1>
+      <formula1>'ion_mobility'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="W2:W1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'matrix_deposition_method'!$A$1:$A$5</formula1>
@@ -1553,6 +1568,43 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1561,86 +1613,49 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B1" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="B3" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="B5" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B6" t="s">
-        <v>258</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B3" t="s">
         <v>265</v>
       </c>
     </row>
@@ -1981,16 +1996,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2">
@@ -1998,13 +2013,13 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DMACA as a new preparation matrix
Closes #19
</commit_message>
<xml_diff>
--- a/maldi/latest/maldi.xlsx
+++ b/maldi/latest/maldi.xlsx
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="380">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -344,6 +344,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000300</t>
   </si>
   <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
+  </si>
+  <si>
     <t>CyCIF</t>
   </si>
   <si>
@@ -449,6 +455,12 @@
     <t>analyte_class</t>
   </si>
   <si>
+    <t>DNA + RNA</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000327</t>
+  </si>
+  <si>
     <t>Chromatin</t>
   </si>
   <si>
@@ -569,6 +581,12 @@
     <t>https://identifiers.org/RRID:SCR_023606</t>
   </si>
   <si>
+    <t>GE Healthcare</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_000004</t>
+  </si>
+  <si>
     <t>Sciex</t>
   </si>
   <si>
@@ -623,6 +641,12 @@
     <t>https://identifiers.org/RRID:SCR_023609</t>
   </si>
   <si>
+    <t>Huron Digital Pathology</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024996</t>
+  </si>
+  <si>
     <t>Illumina</t>
   </si>
   <si>
@@ -692,6 +716,12 @@
     <t>https://identifiers.org/RRID:SCR_023616</t>
   </si>
   <si>
+    <t>PhenoImager Fusion</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023274</t>
+  </si>
+  <si>
     <t>DM6 B</t>
   </si>
   <si>
@@ -752,6 +782,12 @@
     <t>https://identifiers.org/RRID:SCR_023615</t>
   </si>
   <si>
+    <t>TissueScope LE Slide Scanner</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_024995</t>
+  </si>
+  <si>
     <t>VS200 Slide Scanner</t>
   </si>
   <si>
@@ -836,6 +872,12 @@
     <t>https://identifiers.org/RRID:SCR_023617</t>
   </si>
   <si>
+    <t>Aperio AT2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_021256</t>
+  </si>
+  <si>
     <t>MIBIscope</t>
   </si>
   <si>
@@ -1148,6 +1190,12 @@
     <t>preparation_instrument_vendor</t>
   </si>
   <si>
+    <t>Roche Diagnostics</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025096</t>
+  </si>
+  <si>
     <t>HTX Technologies</t>
   </si>
   <si>
@@ -1175,6 +1223,12 @@
     <t>https://identifiers.org/RRID:SCR_023729</t>
   </si>
   <si>
+    <t>EVOS M7000</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025070</t>
+  </si>
+  <si>
     <t>Chromium Controller</t>
   </si>
   <si>
@@ -1211,6 +1265,18 @@
     <t>https://identifiers.org/RRID:SCR_023731</t>
   </si>
   <si>
+    <t>Discovery Ultra</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025097</t>
+  </si>
+  <si>
+    <t>ST5020 Multistainer</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_025021</t>
+  </si>
+  <si>
     <t>Chromium iX</t>
   </si>
   <si>
@@ -1274,6 +1340,12 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_64340</t>
   </si>
   <si>
+    <t>DMACA (4-(dimethylamino)cinnamic acid)</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/MESH/C481008</t>
+  </si>
+  <si>
     <t>analysis_protocol_doi</t>
   </si>
   <si>
@@ -1295,7 +1367,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2024-01-29T14:15:13-08:00</t>
+    <t>2024-03-21T14:23:20-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1447,102 +1519,102 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>226</v>
+        <v>240</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>241</v>
+        <v>255</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>268</v>
+        <v>282</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>276</v>
+        <v>290</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>277</v>
+        <v>291</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>278</v>
+        <v>292</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>279</v>
+        <v>293</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>292</v>
+        <v>306</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>331</v>
+        <v>353</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>346</v>
+        <v>370</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>347</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AB2" t="s" s="29">
-        <v>348</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="21">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$33</formula1>
+      <formula1>'dataset_type'!$A$1:$A$34</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'analyte_class'!$A$1:$A$11</formula1>
+      <formula1>'analyte_class'!$A$1:$A$12</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="F2:F1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_targeted'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="G2:G1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_vendor'!$A$1:$A$19</formula1>
+      <formula1>'acquisition_instrument_vendor'!$A$1:$A$21</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$45</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$48</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1590,13 +1662,13 @@
       <formula1>'matrix_deposition_method'!$A$1:$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="X2:X1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_vendor'!$A$1:$A$7</formula1>
+      <formula1>'preparation_instrument_vendor'!$A$1:$A$9</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Y2:Y1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_instrument_model'!$A$1:$A$14</formula1>
+      <formula1>'preparation_instrument_model'!$A$1:$A$17</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'preparation_matrix'!$A$1:$A$7</formula1>
+      <formula1>'preparation_matrix'!$A$1:$A$8</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1615,26 +1687,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>263</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>265</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>267</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -1652,26 +1724,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>269</v>
+        <v>283</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>270</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>271</v>
+        <v>285</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>272</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>273</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>274</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -1689,50 +1761,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>281</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>283</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>284</v>
+        <v>298</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>285</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>287</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>289</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>291</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -1750,42 +1822,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>293</v>
+        <v>307</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>294</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>296</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>297</v>
+        <v>311</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>298</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>300</v>
+        <v>314</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>301</v>
+        <v>315</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>302</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -1795,7 +1867,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1803,58 +1875,74 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>296</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>304</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>305</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>307</v>
+        <v>319</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>125</v>
+        <v>320</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>126</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>309</v>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>131</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -1864,7 +1952,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1872,114 +1960,138 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>296</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>312</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>313</v>
+        <v>329</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>314</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>204</v>
+        <v>331</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>205</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>316</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>317</v>
+        <v>333</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>318</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>320</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>322</v>
+        <v>338</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>324</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>325</v>
+        <v>341</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>326</v>
+        <v>342</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>327</v>
+        <v>343</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>328</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>330</v>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>347</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>349</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>351</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -1989,7 +2101,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1997,58 +2109,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>332</v>
+        <v>354</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>333</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>334</v>
+        <v>356</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>335</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>336</v>
+        <v>358</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>337</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>338</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>339</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>341</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>342</v>
+        <v>364</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>343</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>344</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>345</v>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>368</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2072,30 +2192,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>349</v>
+        <v>373</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>350</v>
+        <v>374</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>352</v>
+        <v>376</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>354</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>351</v>
+        <v>375</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>355</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -2105,7 +2225,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2375,6 +2495,14 @@
         <v>69</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2382,7 +2510,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2390,90 +2518,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2491,12 +2627,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2506,7 +2642,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2514,154 +2650,170 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>134</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>141</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2671,7 +2823,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2679,362 +2831,386 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>139</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>153</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>181</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>191</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>193</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>195</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>199</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>209</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>211</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>213</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>215</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>217</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>225</v>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>234</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>236</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>238</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3052,42 +3228,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>228</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>229</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>233</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>237</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3105,26 +3281,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>230</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>231</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>233</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>234</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>235</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -3142,50 +3318,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>244</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>246</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>248</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>250</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>252</v>
+        <v>266</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>253</v>
+        <v>267</v>
       </c>
     </row>
     <row r="7">
@@ -3193,31 +3369,31 @@
         <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>254</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>256</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>257</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>258</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>260</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added timsTOF FleX and timsTOF FleX MALDI-2
Closes #86
</commit_message>
<xml_diff>
--- a/maldi/latest/maldi.xlsx
+++ b/maldi/latest/maldi.xlsx
@@ -234,7 +234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="446">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -974,6 +974,18 @@
     <t>https://identifiers.org/RRID:SCR_021660</t>
   </si>
   <si>
+    <t>timsTOF FleX</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_026925</t>
+  </si>
+  <si>
+    <t>timsTOF FleX MALDI-2</t>
+  </si>
+  <si>
+    <t>https://identifiers.org/RRID:SCR_023615</t>
+  </si>
+  <si>
     <t>NanoZoomer S210</t>
   </si>
   <si>
@@ -1043,7 +1055,7 @@
     <t>MALDI timsTOF Flex Prototype</t>
   </si>
   <si>
-    <t>https://identifiers.org/RRID:SCR_023615</t>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000433</t>
   </si>
   <si>
     <t>TissueScope LE Slide Scanner</t>
@@ -1553,7 +1565,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-04-24T10:50:17-07:00</t>
+    <t>2025-05-12T09:55:58-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1717,64 +1729,64 @@
         <v>175</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2">
@@ -1782,7 +1794,7 @@
         <v>44</v>
       </c>
       <c r="AB2" t="s" s="29">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -1800,7 +1812,7 @@
       <formula1>'acquisition_instrument_vendor'!$A$1:$A$26</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="H2:H1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'acquisition_instrument_model'!$A$1:$A$66</formula1>
+      <formula1>'acquisition_instrument_model'!$A$1:$A$68</formula1>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" sqref="I2:I1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="Value should be greater than 0" showErrorMessage="true">
       <formula1>0</formula1>
@@ -1873,26 +1885,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -1910,26 +1922,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>350</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>352</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -1947,50 +1959,50 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>367</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>369</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -2008,10 +2020,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
@@ -2024,26 +2036,26 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2093,18 +2105,18 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>385</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7">
@@ -2125,10 +2137,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -2146,10 +2158,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2">
@@ -2162,10 +2174,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4">
@@ -2178,10 +2190,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6">
@@ -2194,98 +2206,98 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>398</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -2303,66 +2315,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -2386,16 +2398,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2">
@@ -2403,13 +2415,13 @@
         <v>44</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -3145,7 +3157,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3601,26 +3613,26 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>149</v>
+        <v>288</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>150</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>290</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>291</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60">
@@ -3677,6 +3689,22 @@
       </c>
       <c r="B66" t="s" s="0">
         <v>305</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>306</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>308</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -3694,42 +3722,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -3747,26 +3775,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>315</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3784,42 +3812,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>326</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>330</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>332</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6">
@@ -3827,7 +3855,7 @@
         <v>44</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7">
@@ -3835,31 +3863,31 @@
         <v>12</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>334</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>336</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>338</v>
+        <v>342</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>